<commit_message>
Update V2.4: Logica de Permuta Multi-Pass (Qualquer Ordem)
</commit_message>
<xml_diff>
--- a/inputs/permutas.xlsx
+++ b/inputs/permutas.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>Data</t>
   </si>
@@ -26,6 +26,9 @@
   </si>
   <si>
     <t>2025-12-01</t>
+  </si>
+  <si>
+    <t>Marcos</t>
   </si>
   <si>
     <t>João</t>
@@ -402,7 +405,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -435,6 +438,17 @@
         <v>5</v>
       </c>
     </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Release V2.7: Layout Centralizado e Tabela de Permutas no Rodape
</commit_message>
<xml_diff>
--- a/inputs/permutas.xlsx
+++ b/inputs/permutas.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Data</t>
   </si>
@@ -26,9 +26,6 @@
   </si>
   <si>
     <t>2025-12-01</t>
-  </si>
-  <si>
-    <t>Marcos</t>
   </si>
   <si>
     <t>João</t>
@@ -405,7 +402,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -438,17 +435,6 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>